<commit_message>
Added functionality to allow users adding columns.
</commit_message>
<xml_diff>
--- a/Excel-CustomXMLPart-Demo/Copy of TestBook_mszcool_testing.xlsx
+++ b/Excel-CustomXMLPart-Demo/Copy of TestBook_mszcool_testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Id</t>
   </si>
@@ -69,22 +69,16 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>Israel</t>
+    <t>NewCol</t>
+  </si>
+  <si>
+    <t>asöldkfj</t>
+  </si>
+  <si>
+    <t>lasdkjf</t>
+  </si>
+  <si>
+    <t>asldkfj</t>
   </si>
 </sst>
 </file>
@@ -197,19 +191,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -223,14 +235,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB4CB415-F013-4562-8248-7F9ED21D360A}" name="PersonsTable" displayName="PersonsTable" ref="B3:F8" totalsRowShown="0">
-  <autoFilter ref="B3:F8" xr:uid="{378B6608-91C4-40F1-B483-81D9B4A13BF1}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB4CB415-F013-4562-8248-7F9ED21D360A}" name="PersonsTable" displayName="PersonsTable" ref="B3:G6" totalsRowShown="0">
+  <autoFilter ref="B3:G6" xr:uid="{378B6608-91C4-40F1-B483-81D9B4A13BF1}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7B2D722C-4308-47FB-9682-ADF81A7D6478}" name="Id"/>
     <tableColumn id="2" xr3:uid="{FAC5835A-7F4C-422E-86E7-72C2117F2D0F}" name="Firstname"/>
     <tableColumn id="3" xr3:uid="{C9CFAD97-9BF1-4A59-AE2C-531751BD866F}" name="Lastname"/>
     <tableColumn id="4" xr3:uid="{322A240F-896A-4BA3-AAA4-E08C17ACAB17}" name="Age"/>
     <tableColumn id="5" xr3:uid="{928979FF-D4BD-4C34-B05E-5E21D4D11FE0}" name="Country"/>
+    <tableColumn id="6" xr3:uid="{3E3362FC-F678-4129-B92F-04E9597FDAEA}" name="NewCol" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -536,7 +549,7 @@
   <wetp:taskpane dockstate="right" visibility="0" width="612" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
-  <wetp:taskpane dockstate="" visibility="0" width="350" row="4">
+  <wetp:taskpane dockstate="" visibility="0" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
@@ -724,10 +737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF6F59D-A0E0-4925-9FC1-114F182303FE}">
-  <dimension ref="B3:F8"/>
+  <dimension ref="B3:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +754,7 @@
     <col min="7" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -757,8 +770,11 @@
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -774,8 +790,11 @@
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -791,8 +810,11 @@
       <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -808,39 +830,8 @@
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5">
-        <v>40</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5">
-        <v>50</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -928,6 +919,7 @@
     <lastname>aa</lastname>
     <age>10</age>
     <country>India</country>
+    <newcol>asöldkfj</newcol>
   </Person>
   <Person xmlns="" ID="2">
     <id>2</id>
@@ -935,6 +927,7 @@
     <lastname>bb</lastname>
     <age>20</age>
     <country>Austria</country>
+    <newcol>lasdkjf</newcol>
   </Person>
   <Person xmlns="" ID="3">
     <id>3</id>
@@ -942,20 +935,7 @@
     <lastname>cc</lastname>
     <age>30</age>
     <country>Germany</country>
-  </Person>
-  <Person xmlns="" ID="4">
-    <id>4</id>
-    <firstname>d</firstname>
-    <lastname>dd</lastname>
-    <age>40</age>
-    <country>United States</country>
-  </Person>
-  <Person xmlns="" ID="5">
-    <id>5</id>
-    <firstname>e</firstname>
-    <lastname>ee</lastname>
-    <age>50</age>
-    <country>Israel</country>
+    <newcol>asldkfj</newcol>
   </Person>
 </PersonsData>
 </file>
@@ -969,7 +949,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E636AF1F-C02B-42E8-B981-9A375ADF6AC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48AEB3F8-B527-4B00-8D6F-B109AE2991BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="SapPrototypeTest"/>
     <ds:schemaRef ds:uri=""/>

</xml_diff>